<commit_message>
Added my ml projects
</commit_message>
<xml_diff>
--- a/Excel/Clean_recharge_data.xlsx
+++ b/Excel/Clean_recharge_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITCS\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AIML\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1376A1A6-42DF-486A-859E-652BD6571A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B858B2BA-85A0-4557-83FA-3A62F34F85A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9D5D9271-BA89-4C6C-8D28-2D14D6774CFF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{57EA3B9B-A84B-4175-BF00-4FAD2A6F25C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,12 +106,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,12 +127,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -136,14 +156,14 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -458,21 +478,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3E0398-870B-401E-94E9-51E9AADDACD3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A49DC7-E135-420C-AEA3-9A404D8E59F1}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>101</v>
       </c>
@@ -512,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>102</v>
       </c>
@@ -532,7 +555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>103</v>
       </c>
@@ -552,7 +575,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>105</v>
       </c>
@@ -572,7 +595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>105</v>
       </c>
@@ -592,7 +615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>106</v>
       </c>
@@ -612,7 +635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>106</v>
       </c>
@@ -632,7 +655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>107</v>
       </c>
@@ -652,7 +675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>108</v>
       </c>
@@ -672,7 +695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>109</v>
       </c>
@@ -692,7 +715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>110</v>
       </c>
@@ -712,7 +735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>111</v>
       </c>
@@ -732,7 +755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>112</v>
       </c>
@@ -752,7 +775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>113</v>
       </c>
@@ -772,7 +795,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>114</v>
       </c>
@@ -792,7 +815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>115</v>
       </c>
@@ -814,5 +837,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>